<commit_message>
Added tug parsing, charging nodes, base functionality of tugs and displaying tugs
</commit_message>
<xml_diff>
--- a/edges.xlsx
+++ b/edges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6aaedf7c31cb3db/Documenten/TA_ABMS/code_student_versie10_09/code_student_versie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codings\py\AEagentbased\Agent_based\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{8619D402-E8AF-48C7-ADA5-03BC2EAEC118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D40FE721-0762-4D8D-A5B7-2D189D2270B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D409DAA-E807-49AB-AE33-CF05F2DA9970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1DB0F0EF-2216-4628-B5EE-950EADE27966}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1DB0F0EF-2216-4628-B5EE-950EADE27966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,19 +18,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -397,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78937278-08B5-42DE-93BA-E4F0710E1C5E}">
-  <dimension ref="A1:C253"/>
+  <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="G237" sqref="G237"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3188,6 +3179,50 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>108</v>
+      </c>
+      <c r="B254">
+        <v>109</v>
+      </c>
+      <c r="C254">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>109</v>
+      </c>
+      <c r="B255">
+        <v>108</v>
+      </c>
+      <c r="C255">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>107</v>
+      </c>
+      <c r="B256">
+        <v>110</v>
+      </c>
+      <c r="C256">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>110</v>
+      </c>
+      <c r="B257">
+        <v>107</v>
+      </c>
+      <c r="C257">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bidding and charging is implemented.
</commit_message>
<xml_diff>
--- a/edges.xlsx
+++ b/edges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codings\py\AEagentbased\Agent_based\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D409DAA-E807-49AB-AE33-CF05F2DA9970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720917AE-21E8-4A56-ABC8-08A75D24E935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1DB0F0EF-2216-4628-B5EE-950EADE27966}"/>
   </bookViews>
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78937278-08B5-42DE-93BA-E4F0710E1C5E}">
   <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E258" sqref="E258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="B254">
         <v>109</v>
@@ -3195,7 +3195,7 @@
         <v>109</v>
       </c>
       <c r="B255">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="C255">
         <v>0.5</v>

</xml_diff>

<commit_message>
added unit test, changed simulation logic
</commit_message>
<xml_diff>
--- a/edges.xlsx
+++ b/edges.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codings\py\AEagentbased\Agent_based\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Agent_based\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720917AE-21E8-4A56-ABC8-08A75D24E935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79061E61-6904-4FB4-8DC7-69C75BE2419D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1DB0F0EF-2216-4628-B5EE-950EADE27966}"/>
+    <workbookView xWindow="3000" yWindow="1090" windowWidth="14400" windowHeight="8170" xr2:uid="{1DB0F0EF-2216-4628-B5EE-950EADE27966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -132,7 +132,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -238,7 +238,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -380,7 +380,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -390,13 +390,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78937278-08B5-42DE-93BA-E4F0710E1C5E}">
   <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E258" sqref="E258"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="E255" sqref="E255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3</v>
       </c>
@@ -418,7 +418,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -429,7 +429,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
@@ -440,7 +440,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -451,7 +451,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -462,7 +462,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -473,7 +473,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -484,7 +484,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -495,7 +495,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>6</v>
       </c>
@@ -506,7 +506,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>7</v>
       </c>
@@ -517,7 +517,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>7</v>
       </c>
@@ -528,7 +528,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>8</v>
       </c>
@@ -539,7 +539,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>8</v>
       </c>
@@ -550,7 +550,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>8</v>
       </c>
@@ -561,7 +561,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>9</v>
       </c>
@@ -572,7 +572,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>9</v>
       </c>
@@ -583,7 +583,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9</v>
       </c>
@@ -594,7 +594,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>10</v>
       </c>
@@ -605,7 +605,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>10</v>
       </c>
@@ -616,7 +616,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>10</v>
       </c>
@@ -627,7 +627,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>11</v>
       </c>
@@ -638,7 +638,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>11</v>
       </c>
@@ -649,7 +649,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>11</v>
       </c>
@@ -660,7 +660,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>12</v>
       </c>
@@ -671,7 +671,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>12</v>
       </c>
@@ -682,7 +682,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>12</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>13</v>
       </c>
@@ -704,7 +704,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>13</v>
       </c>
@@ -715,7 +715,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>13</v>
       </c>
@@ -726,7 +726,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>14</v>
       </c>
@@ -737,7 +737,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>14</v>
       </c>
@@ -748,7 +748,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>14</v>
       </c>
@@ -759,7 +759,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>15</v>
       </c>
@@ -770,7 +770,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>15</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>15</v>
       </c>
@@ -792,7 +792,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>15</v>
       </c>
@@ -803,7 +803,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>16</v>
       </c>
@@ -814,7 +814,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>16</v>
       </c>
@@ -825,7 +825,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>16</v>
       </c>
@@ -836,7 +836,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>17</v>
       </c>
@@ -847,7 +847,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>17</v>
       </c>
@@ -858,7 +858,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>18</v>
       </c>
@@ -869,7 +869,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>18</v>
       </c>
@@ -880,7 +880,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>18</v>
       </c>
@@ -891,7 +891,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>18</v>
       </c>
@@ -902,7 +902,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>19</v>
       </c>
@@ -913,7 +913,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>19</v>
       </c>
@@ -924,7 +924,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>19</v>
       </c>
@@ -935,7 +935,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>19</v>
       </c>
@@ -946,7 +946,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>20</v>
       </c>
@@ -957,7 +957,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>20</v>
       </c>
@@ -968,7 +968,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>20</v>
       </c>
@@ -979,7 +979,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>20</v>
       </c>
@@ -990,7 +990,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>21</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>21</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>21</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>21</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>22</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>22</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>22</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>22</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>23</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>23</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>24</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>24</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>24</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>25</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>25</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>25</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>26</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>26</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>26</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>26</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>27</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>27</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>27</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>27</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>28</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>28</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>28</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>29</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>29</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>30</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>30</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>30</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>31</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>31</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>31</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>32</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>32</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>32</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>33</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>33</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>39</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>39</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>40</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>40</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>41</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>41</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>42</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>42</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>43</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>43</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>44</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>44</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>45</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>45</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>46</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>46</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>47</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>47</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>48</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>48</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>49</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>49</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>50</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>50</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>51</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>51</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>52</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>52</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>53</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>53</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>54</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>54</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>55</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>55</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>56</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>56</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>57</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>57</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>58</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>58</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>59</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>59</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>60</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>60</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>61</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>61</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>62</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>62</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>63</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>63</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>64</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>64</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>65</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>65</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>66</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>66</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>67</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>67</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>68</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>68</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>69</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>69</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>70</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>70</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>71</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>71</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>72</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>72</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>73</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>73</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>74</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>74</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>75</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>75</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>76</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>76</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>77</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>77</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>78</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>78</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>79</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>79</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>80</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>80</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>81</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>81</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>82</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>82</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>83</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>83</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>84</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>84</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>85</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>85</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>86</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>86</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>87</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>87</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>88</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>88</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>89</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>89</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>90</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>90</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>91</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>91</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>1</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>95</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>2</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>96</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>30</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>92</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>31</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>93</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>32</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>94</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>95</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>4</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>96</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>5</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>92</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>34</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>93</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>35</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>94</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>36</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>29</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>99</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>33</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>100</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>99</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>97</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>100</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>98</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>37</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>101</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>38</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>102</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>101</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>11</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>102</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>12</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>17</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>103</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>104</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>105</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>28</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>106</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>107</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>108</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>103</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>104</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>105</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>24</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>106</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>107</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>108</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>23</v>
       </c>
@@ -3179,9 +3179,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="B254">
         <v>109</v>
@@ -3190,18 +3190,18 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>109</v>
       </c>
       <c r="B255">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="C255">
         <v>0.5</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>107</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
Added Tim's simulation codes
</commit_message>
<xml_diff>
--- a/edges.xlsx
+++ b/edges.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Agent_based\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tim\Documents\TU\Master\AE4422-20 Agent-based Modelling and Simulation in Airtransport\Code\Agent_based-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79061E61-6904-4FB4-8DC7-69C75BE2419D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CEA69D-191E-440A-A680-74046649CC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1090" windowWidth="14400" windowHeight="8170" xr2:uid="{1DB0F0EF-2216-4628-B5EE-950EADE27966}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1DB0F0EF-2216-4628-B5EE-950EADE27966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,13 +390,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78937278-08B5-42DE-93BA-E4F0710E1C5E}">
   <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="E255" sqref="E255"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="A255" sqref="A255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3</v>
       </c>
@@ -418,7 +418,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -429,7 +429,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -440,7 +440,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -451,7 +451,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -462,7 +462,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -473,7 +473,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -484,7 +484,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -495,7 +495,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -506,7 +506,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -517,7 +517,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7</v>
       </c>
@@ -528,7 +528,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -539,7 +539,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
@@ -550,7 +550,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -561,7 +561,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -572,7 +572,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9</v>
       </c>
@@ -583,7 +583,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>9</v>
       </c>
@@ -594,7 +594,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10</v>
       </c>
@@ -605,7 +605,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10</v>
       </c>
@@ -616,7 +616,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10</v>
       </c>
@@ -627,7 +627,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>11</v>
       </c>
@@ -638,7 +638,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>11</v>
       </c>
@@ -649,7 +649,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>11</v>
       </c>
@@ -660,7 +660,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12</v>
       </c>
@@ -671,7 +671,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12</v>
       </c>
@@ -682,7 +682,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>12</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>13</v>
       </c>
@@ -704,7 +704,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>13</v>
       </c>
@@ -715,7 +715,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>13</v>
       </c>
@@ -726,7 +726,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>14</v>
       </c>
@@ -737,7 +737,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>14</v>
       </c>
@@ -748,7 +748,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>14</v>
       </c>
@@ -759,7 +759,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>15</v>
       </c>
@@ -770,7 +770,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>15</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>15</v>
       </c>
@@ -792,7 +792,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>15</v>
       </c>
@@ -803,7 +803,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>16</v>
       </c>
@@ -814,7 +814,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>16</v>
       </c>
@@ -825,7 +825,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>16</v>
       </c>
@@ -836,7 +836,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>17</v>
       </c>
@@ -847,7 +847,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>17</v>
       </c>
@@ -858,7 +858,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>18</v>
       </c>
@@ -869,7 +869,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>18</v>
       </c>
@@ -880,7 +880,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>18</v>
       </c>
@@ -891,7 +891,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>18</v>
       </c>
@@ -902,7 +902,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>19</v>
       </c>
@@ -913,7 +913,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>19</v>
       </c>
@@ -924,7 +924,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>19</v>
       </c>
@@ -935,7 +935,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>19</v>
       </c>
@@ -946,7 +946,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>20</v>
       </c>
@@ -957,7 +957,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>20</v>
       </c>
@@ -968,7 +968,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>20</v>
       </c>
@@ -979,7 +979,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>20</v>
       </c>
@@ -990,7 +990,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>21</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>21</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>21</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>21</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>22</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>22</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>22</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>22</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>23</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>23</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>24</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>24</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>24</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>25</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>25</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>25</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>26</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>26</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>26</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>26</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>27</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>27</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>27</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>27</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>28</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>28</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>28</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>29</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>29</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>30</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>30</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>30</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>31</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>31</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>31</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>32</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>32</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>32</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>33</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>33</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>39</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>39</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>40</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>40</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>41</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>41</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>42</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>42</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>43</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>43</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>44</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>44</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>45</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>45</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>46</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>46</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>47</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>47</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>48</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>48</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>49</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>49</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>50</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>50</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>51</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>51</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>52</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>52</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>53</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>53</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>54</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>54</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>55</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>55</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>56</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>56</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>57</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>57</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>58</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>58</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>59</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>59</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>60</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>60</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>61</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>61</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>62</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>62</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>63</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>63</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>64</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>64</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>65</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>65</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>66</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>66</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>67</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>67</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>68</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>68</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>69</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>69</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>70</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>70</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>71</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>71</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>72</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>72</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>73</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>73</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>74</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>74</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>75</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>75</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>76</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>76</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>77</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>77</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>78</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>78</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>79</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>79</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>80</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>80</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>81</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>81</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>82</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>82</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>83</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>83</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>84</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>84</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>85</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>85</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>86</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>86</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>87</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>87</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>88</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>88</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>89</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>89</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>90</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>90</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>91</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>91</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>1</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>95</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>2</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>96</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>30</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>92</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>31</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>93</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>32</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>94</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>95</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>4</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>96</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>5</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>92</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>34</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>93</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>35</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>94</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>36</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>29</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>99</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>33</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>100</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>99</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>97</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>100</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>98</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>37</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>101</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>38</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>102</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>101</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>11</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>102</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>12</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>17</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>103</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>104</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>105</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>28</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>106</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>107</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>108</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>103</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>104</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>105</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>24</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>106</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>107</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>108</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>23</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>104</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>109</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>107</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>110</v>
       </c>

</xml_diff>